<commit_message>
record dataset with specificity question genreated
</commit_message>
<xml_diff>
--- a/exp_output/eos-sft_musique_propagator_text_seen_w-atomq/musique/mend_eval_loss=clm_input=seen_n=1_prompt=no_w-gen_wo-icl.xlsx
+++ b/exp_output/eos-sft_musique_propagator_text_seen_w-atomq/musique/mend_eval_loss=clm_input=seen_n=1_prompt=no_w-gen_wo-icl.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
           <t>[Q][A] Acc PM</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>llm_accuracy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -596,6 +601,9 @@
       <c r="R2" t="n">
         <v>0.5</v>
       </c>
+      <c r="S2" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -668,6 +676,9 @@
       <c r="R3" t="n">
         <v>0.529411792755127</v>
       </c>
+      <c r="S3" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -739,6 +750,9 @@
       </c>
       <c r="R4" t="n">
         <v>0.4375</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>